<commit_message>
execução de ponta a ponta
</commit_message>
<xml_diff>
--- a/faturas.xlsx
+++ b/faturas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -510,35 +510,146 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>0003340074</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>26/08/2025</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>19/08/2025</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>908,91</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>030.663.374</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>34191.09123 70053.972934 85972.140009 1 11850000090891</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>08.2025 - Energisa - Inst 103340074-8.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>0000893797</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>16/09/2025</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>07/08/2025</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0,00</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>014.775.807</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>74593.10046 27628.019005 01374.441762 7 12060000000000</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>08.2025 - Energisa - Inst 8893797-1.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>893797</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>25/09/2025</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>18/09/2025</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>29,53</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>005.598.958</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>83650000000-2 29530012000-9 72680172025-1 09200002019-5</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>09.2025 - Energisa - Inst 8893797-1 Desligamento.pdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>0002872694</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>11/07/2025</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>10/06/2025</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>380,50</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>028.722.338</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>34191.09115 38025.002932 85972.140009 1 11390000038050</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>1 2872694.pdf</t>
         </is>

</xml_diff>